<commit_message>
Fix tỉ lệ lỗi excel
</commit_message>
<xml_diff>
--- a/temp/Sokatu/Resources/ExportExcel.xlsx
+++ b/temp/Sokatu/Resources/ExportExcel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="11040"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,7 +221,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,7 +256,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,10 +468,10 @@
   <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>